<commit_message>
update example input and output files
</commit_message>
<xml_diff>
--- a/sample_data/workbook_1.xlsx
+++ b/sample_data/workbook_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Private\Python\perf_sum_from_xls\sample_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Private\Python\xls_rows_cols_to_csv\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777DD9A0-6396-4E56-922A-911C83B460DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E6A440-E3FD-40E9-ACBF-B6BC85CB84DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26385" yWindow="1605" windowWidth="21450" windowHeight="8130" activeTab="1" xr2:uid="{0D2FD608-69DA-4D25-9957-4D858AB48404}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="15345" xr2:uid="{0D2FD608-69DA-4D25-9957-4D858AB48404}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet_A" sheetId="1" r:id="rId1"/>
@@ -146,7 +146,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -203,9 +203,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -543,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E314C98C-F3D9-4325-98C2-A55C646EAAA4}">
-  <dimension ref="B1:L12"/>
+  <dimension ref="B1:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -614,28 +614,22 @@
         <v>19</v>
       </c>
       <c r="E4" s="7">
-        <f>E3*E8</f>
-        <v>25.72005872986951</v>
+        <v>25.720099999999999</v>
       </c>
       <c r="F4" s="7">
-        <f t="shared" ref="F4:J4" si="0">F3*F8</f>
-        <v>51.440117459739021</v>
+        <v>51.440100000000001</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" si="0"/>
-        <v>77.160176189608535</v>
+        <v>77.160200000000003</v>
       </c>
       <c r="H4" s="7">
-        <f t="shared" si="0"/>
-        <v>12.860029364934755</v>
+        <v>12.86</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" si="0"/>
-        <v>25.72005872986951</v>
+        <v>25.720099999999999</v>
       </c>
       <c r="J4" s="7">
-        <f t="shared" si="0"/>
-        <v>38.580088094804267</v>
+        <v>38.580100000000002</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
@@ -646,22 +640,22 @@
         <v>20</v>
       </c>
       <c r="E5" s="3">
-        <v>0.92202765154903898</v>
+        <v>0.92200000000000004</v>
       </c>
       <c r="F5" s="3">
-        <v>0.92202765154903898</v>
+        <v>0.92200000000000004</v>
       </c>
       <c r="G5" s="3">
-        <v>0.92202765154903898</v>
+        <v>0.92200000000000004</v>
       </c>
       <c r="H5" s="3">
-        <v>0.92202765154903898</v>
+        <v>0.92200000000000004</v>
       </c>
       <c r="I5" s="3">
-        <v>0.92202765154903898</v>
+        <v>0.92200000000000004</v>
       </c>
       <c r="J5" s="3">
-        <v>0.92202765154903898</v>
+        <v>0.92200000000000004</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
@@ -672,22 +666,22 @@
         <v>21</v>
       </c>
       <c r="E6" s="3">
-        <v>1.2818360225868188</v>
+        <v>1.2818000000000001</v>
       </c>
       <c r="F6" s="3">
-        <v>1.2818360225868222</v>
+        <v>1.2818000000000001</v>
       </c>
       <c r="G6" s="3">
-        <v>1.2818360225868206</v>
+        <v>1.2818000000000001</v>
       </c>
       <c r="H6" s="3">
-        <v>1.2818360225868184</v>
+        <v>1.2818000000000001</v>
       </c>
       <c r="I6" s="3">
-        <v>1.2818360225868204</v>
+        <v>1.2818000000000001</v>
       </c>
       <c r="J6" s="3">
-        <v>1.2818360225868188</v>
+        <v>1.2818000000000001</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
@@ -698,22 +692,22 @@
         <v>22</v>
       </c>
       <c r="E7" s="3">
-        <v>28.82960201596325</v>
+        <v>28.829599999999999</v>
       </c>
       <c r="F7" s="3">
-        <v>28.82960201596325</v>
+        <v>28.829599999999999</v>
       </c>
       <c r="G7" s="3">
-        <v>28.82960201596325</v>
+        <v>28.829599999999999</v>
       </c>
       <c r="H7" s="3">
-        <v>28.82960201596325</v>
+        <v>28.829599999999999</v>
       </c>
       <c r="I7" s="3">
-        <v>28.82960201596325</v>
+        <v>28.829599999999999</v>
       </c>
       <c r="J7" s="3">
-        <v>28.82960201596325</v>
+        <v>28.829599999999999</v>
       </c>
       <c r="K7" s="4"/>
     </row>
@@ -725,22 +719,22 @@
         <v>23</v>
       </c>
       <c r="E8" s="3">
-        <v>1.2860029364934755</v>
+        <v>1.286</v>
       </c>
       <c r="F8" s="3">
-        <v>1.2860029364934755</v>
+        <v>1.286</v>
       </c>
       <c r="G8" s="3">
-        <v>1.2860029364934755</v>
+        <v>1.286</v>
       </c>
       <c r="H8" s="3">
-        <v>1.2860029364934755</v>
+        <v>1.286</v>
       </c>
       <c r="I8" s="3">
-        <v>1.2860029364934755</v>
+        <v>1.286</v>
       </c>
       <c r="J8" s="3">
-        <v>1.2860029364934755</v>
+        <v>1.286</v>
       </c>
       <c r="K8" s="4"/>
     </row>
@@ -752,22 +746,22 @@
         <v>24</v>
       </c>
       <c r="E9" s="3">
-        <v>845.10823539588478</v>
+        <v>845.10820000000001</v>
       </c>
       <c r="F9" s="3">
-        <v>844.17967636020614</v>
+        <v>844.17970000000003</v>
       </c>
       <c r="G9" s="3">
-        <v>837.53705529104536</v>
+        <v>837.53710000000001</v>
       </c>
       <c r="H9" s="3">
-        <v>836.87974852332309</v>
+        <v>836.87969999999996</v>
       </c>
       <c r="I9" s="3">
-        <v>778.60456645811212</v>
+        <v>778.6046</v>
       </c>
       <c r="J9" s="3">
-        <v>853.90997668513091</v>
+        <v>853.91</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
@@ -778,22 +772,22 @@
         <v>25</v>
       </c>
       <c r="E10" s="3">
-        <v>102.00255952542544</v>
+        <v>102.0026</v>
       </c>
       <c r="F10" s="3">
-        <v>102.00027623283471</v>
+        <v>102.0003</v>
       </c>
       <c r="G10" s="3">
-        <v>102.00489329996365</v>
+        <v>102.00490000000001</v>
       </c>
       <c r="H10" s="3">
-        <v>102.0154689852215</v>
+        <v>102.0155</v>
       </c>
       <c r="I10" s="3">
-        <v>101.98878123698714</v>
+        <v>101.9888</v>
       </c>
       <c r="J10" s="3">
-        <v>102.03870905434617</v>
+        <v>102.03870000000001</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
@@ -806,22 +800,22 @@
         <v>26</v>
       </c>
       <c r="E11" s="5">
-        <v>312.46028536145866</v>
+        <v>312.46030000000002</v>
       </c>
       <c r="F11" s="5">
-        <v>312.45863247196939</v>
+        <v>312.45859999999999</v>
       </c>
       <c r="G11" s="3">
-        <v>312.46197476552982</v>
+        <v>312.46199999999999</v>
       </c>
       <c r="H11" s="5">
-        <v>312.46963005954774</v>
+        <v>312.46960000000001</v>
       </c>
       <c r="I11" s="3">
-        <v>312.45031073882421</v>
+        <v>312.45030000000003</v>
       </c>
       <c r="J11" s="5">
-        <v>312.48645040980671</v>
+        <v>312.48649999999998</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
@@ -834,25 +828,106 @@
         <v>27</v>
       </c>
       <c r="E12" s="5">
-        <v>1416.489726437771</v>
+        <v>1416.4897000000001</v>
       </c>
       <c r="F12" s="5">
-        <v>1416.4799350877577</v>
+        <v>1416.4799</v>
       </c>
       <c r="G12" s="3">
-        <v>1416.4997341757085</v>
+        <v>1416.4997000000001</v>
       </c>
       <c r="H12" s="5">
-        <v>1416.5450838752554</v>
+        <v>1416.5451</v>
       </c>
       <c r="I12" s="3">
-        <v>1416.4306402196089</v>
+        <v>1416.4305999999999</v>
       </c>
       <c r="J12" s="5">
-        <v>1416.6447331552624</v>
+        <v>1416.6447000000001</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
+    </row>
+    <row r="17" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E28" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -864,7 +939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9332C861-98A8-435F-91BC-9B6DC7D10A21}">
   <dimension ref="B1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
@@ -998,27 +1073,27 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="8">
-        <f>SUM(E3:E6)</f>
+        <f t="shared" ref="E9:J9" si="0">SUM(E3:E6)</f>
         <v>100</v>
       </c>
       <c r="F9" s="8">
-        <f>SUM(F3:F6)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="G9" s="2">
-        <f>SUM(G3:G6)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="H9" s="8">
-        <f>SUM(H3:H6)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="I9" s="2">
-        <f>SUM(I3:I6)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="J9" s="8">
-        <f>SUM(J3:J6)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>

</xml_diff>